<commit_message>
Update blank building on Parkville campus
</commit_message>
<xml_diff>
--- a/unimelb_parville_url.xlsx
+++ b/unimelb_parville_url.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimelbcloud-my.sharepoint.com/personal/boat_amorntiyanggoon_unimelb_edu_au/Documents/Casual Tasks/URL_extraction/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_52C182F37E3309A243C2F8C6D14E3EF37979390D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58B0CF80-907D-45D5-89D6-521D751BB64A}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2472" yWindow="2472" windowWidth="17280" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="402">
   <si>
     <t>Building name</t>
   </si>
@@ -145,6 +139,9 @@
     <t>Peter Hall Building</t>
   </si>
   <si>
+    <t>Building 161</t>
+  </si>
+  <si>
     <t>Student Pavilion</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
     <t>Chemical Engineering Building 2</t>
   </si>
   <si>
+    <t>Building 168</t>
+  </si>
+  <si>
     <t>Engineering Workshops</t>
   </si>
   <si>
@@ -181,6 +181,9 @@
     <t>Infrastructure Engineering (Block D)</t>
   </si>
   <si>
+    <t>Building 177</t>
+  </si>
+  <si>
     <t>Medical Building</t>
   </si>
   <si>
@@ -199,6 +202,9 @@
     <t>Visitor &amp; Merchandise Centre</t>
   </si>
   <si>
+    <t>Building 189</t>
+  </si>
+  <si>
     <t>John Medley</t>
   </si>
   <si>
@@ -253,6 +259,9 @@
     <t>766 Elizabeth Street</t>
   </si>
   <si>
+    <t>Building 224</t>
+  </si>
+  <si>
     <t>MUS Grandstand</t>
   </si>
   <si>
@@ -271,9 +280,21 @@
     <t>Peter Doherty Institute</t>
   </si>
   <si>
+    <t>Building 249</t>
+  </si>
+  <si>
+    <t>Building 250</t>
+  </si>
+  <si>
+    <t>Building 251</t>
+  </si>
+  <si>
     <t>156-162 Pelham St</t>
   </si>
   <si>
+    <t>Building 253</t>
+  </si>
+  <si>
     <t>Victorian Comprehensive Cancer Centre</t>
   </si>
   <si>
@@ -319,24 +340,54 @@
     <t>Peter McPhee Centre</t>
   </si>
   <si>
+    <t>Building 348</t>
+  </si>
+  <si>
+    <t>Building 352</t>
+  </si>
+  <si>
+    <t>Building 353</t>
+  </si>
+  <si>
     <t>Graduate House</t>
   </si>
   <si>
+    <t>Building 363</t>
+  </si>
+  <si>
+    <t>Building 368</t>
+  </si>
+  <si>
     <t>207-221 Bouverie St</t>
   </si>
   <si>
     <t>University Digitisation Centre</t>
   </si>
   <si>
+    <t>Building 385</t>
+  </si>
+  <si>
     <t>21 Bedford St</t>
   </si>
   <si>
+    <t>Building 388</t>
+  </si>
+  <si>
+    <t>Building 390</t>
+  </si>
+  <si>
+    <t>Building 394</t>
+  </si>
+  <si>
     <t>Veterinary Preclinical Sciences</t>
   </si>
   <si>
     <t>Nancy Millis Building</t>
   </si>
   <si>
+    <t>Building 402</t>
+  </si>
+  <si>
     <t>Ruth Bishop Building</t>
   </si>
   <si>
@@ -365,6 +416,9 @@
   </si>
   <si>
     <t>Centre for Medical Research</t>
+  </si>
+  <si>
+    <t>Building 633</t>
   </si>
   <si>
     <t>Royal Dental Hospital of Melbourne</t>
@@ -1171,8 +1225,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1248,14 +1302,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1302,7 +1348,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1334,27 +1380,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1386,24 +1414,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1579,19 +1589,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A119" sqref="A117:A119"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="40.33203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1602,1544 +1607,1604 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
       <c r="B40" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
       <c r="B46" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
       <c r="B54" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>62</v>
+      </c>
       <c r="B61" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B72" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B79" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>81</v>
+      </c>
       <c r="B80" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B84" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B85" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B86" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>88</v>
+      </c>
       <c r="B87" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>89</v>
+      </c>
       <c r="B88" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>90</v>
+      </c>
       <c r="B89" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B90" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>92</v>
+      </c>
       <c r="B91" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B92" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B93" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B94" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B95" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B97" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B98" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B99" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B100" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B101" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B102" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="B103" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B104" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B105" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="B106" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>108</v>
+      </c>
       <c r="B107" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="s">
+        <v>109</v>
+      </c>
       <c r="B108" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>110</v>
+      </c>
       <c r="B109" t="s">
-        <v>223</v>
+        <v>243</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="B110" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
+        <v>112</v>
+      </c>
       <c r="B111" t="s">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
+        <v>113</v>
+      </c>
       <c r="B112" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="B113" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B114" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>116</v>
+      </c>
       <c r="B115" t="s">
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="B116" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>118</v>
+      </c>
       <c r="B117" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>119</v>
+      </c>
       <c r="B118" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>120</v>
+      </c>
       <c r="B119" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="B120" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="B121" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" t="s">
+        <v>123</v>
+      </c>
       <c r="B122" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="B123" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="B124" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="B125" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="B126" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="B127" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="B128" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="B129" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="B130" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="B131" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="B132" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" t="s">
+        <v>134</v>
+      </c>
       <c r="B133" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="B134" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>381</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="C12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="C13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="C14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="C15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="C16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="C17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="C18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="C20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="C21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="C22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="C23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="C25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="C26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="C27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="C28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="C29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="C30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="C31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="C32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="C33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="C34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="C35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="C37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="C38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="C39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="C40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="C41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="C42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="C43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="C44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="C45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="C46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="C47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="C48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="C49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="C50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="C51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="C52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="C53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="C54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="C55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="C56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="C57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="C58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="C59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="C60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="C61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="C62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="C63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="C64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="C65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="C66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="C67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="C68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="C69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="C70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="C71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="C72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="C73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="C74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="C75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="C76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="C77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="C78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="C79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="C80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="C81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="C82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="C83" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="C84" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="C85" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="C86" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="C87" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="C88" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="C89" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="C90" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="C91" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="C92" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="C93" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="C94" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="C95" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="C96" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="C97" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="C98" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="C99" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="C100" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="C101" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="C102" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="C103" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="C104" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="C105" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="C106" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="C107" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="C108" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="C109" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="C110" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="C111" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="C112" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="C113" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="C114" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="C115" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="C116" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="C117" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="C118" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="C119" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="C120" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="C121" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="C122" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="C123" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="C124" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="C125" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="C126" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="C127" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="C128" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="C129" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="C130" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="C131" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="C132" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="C133" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="C134" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
+    <hyperlink ref="C13" r:id="rId12"/>
+    <hyperlink ref="C14" r:id="rId13"/>
+    <hyperlink ref="C15" r:id="rId14"/>
+    <hyperlink ref="C16" r:id="rId15"/>
+    <hyperlink ref="C17" r:id="rId16"/>
+    <hyperlink ref="C18" r:id="rId17"/>
+    <hyperlink ref="C19" r:id="rId18"/>
+    <hyperlink ref="C20" r:id="rId19"/>
+    <hyperlink ref="C21" r:id="rId20"/>
+    <hyperlink ref="C22" r:id="rId21"/>
+    <hyperlink ref="C23" r:id="rId22"/>
+    <hyperlink ref="C24" r:id="rId23"/>
+    <hyperlink ref="C25" r:id="rId24"/>
+    <hyperlink ref="C26" r:id="rId25"/>
+    <hyperlink ref="C27" r:id="rId26"/>
+    <hyperlink ref="C28" r:id="rId27"/>
+    <hyperlink ref="C29" r:id="rId28"/>
+    <hyperlink ref="C30" r:id="rId29"/>
+    <hyperlink ref="C31" r:id="rId30"/>
+    <hyperlink ref="C32" r:id="rId31"/>
+    <hyperlink ref="C33" r:id="rId32"/>
+    <hyperlink ref="C34" r:id="rId33"/>
+    <hyperlink ref="C35" r:id="rId34"/>
+    <hyperlink ref="C36" r:id="rId35"/>
+    <hyperlink ref="C37" r:id="rId36"/>
+    <hyperlink ref="C38" r:id="rId37"/>
+    <hyperlink ref="C39" r:id="rId38"/>
+    <hyperlink ref="C40" r:id="rId39"/>
+    <hyperlink ref="C41" r:id="rId40"/>
+    <hyperlink ref="C42" r:id="rId41"/>
+    <hyperlink ref="C43" r:id="rId42"/>
+    <hyperlink ref="C44" r:id="rId43"/>
+    <hyperlink ref="C45" r:id="rId44"/>
+    <hyperlink ref="C46" r:id="rId45"/>
+    <hyperlink ref="C47" r:id="rId46"/>
+    <hyperlink ref="C48" r:id="rId47"/>
+    <hyperlink ref="C49" r:id="rId48"/>
+    <hyperlink ref="C50" r:id="rId49"/>
+    <hyperlink ref="C51" r:id="rId50"/>
+    <hyperlink ref="C52" r:id="rId51"/>
+    <hyperlink ref="C53" r:id="rId52"/>
+    <hyperlink ref="C54" r:id="rId53"/>
+    <hyperlink ref="C55" r:id="rId54"/>
+    <hyperlink ref="C56" r:id="rId55"/>
+    <hyperlink ref="C57" r:id="rId56"/>
+    <hyperlink ref="C58" r:id="rId57"/>
+    <hyperlink ref="C59" r:id="rId58"/>
+    <hyperlink ref="C60" r:id="rId59"/>
+    <hyperlink ref="C61" r:id="rId60"/>
+    <hyperlink ref="C62" r:id="rId61"/>
+    <hyperlink ref="C63" r:id="rId62"/>
+    <hyperlink ref="C64" r:id="rId63"/>
+    <hyperlink ref="C65" r:id="rId64"/>
+    <hyperlink ref="C66" r:id="rId65"/>
+    <hyperlink ref="C67" r:id="rId66"/>
+    <hyperlink ref="C68" r:id="rId67"/>
+    <hyperlink ref="C69" r:id="rId68"/>
+    <hyperlink ref="C70" r:id="rId69"/>
+    <hyperlink ref="C71" r:id="rId70"/>
+    <hyperlink ref="C72" r:id="rId71"/>
+    <hyperlink ref="C73" r:id="rId72"/>
+    <hyperlink ref="C74" r:id="rId73"/>
+    <hyperlink ref="C75" r:id="rId74"/>
+    <hyperlink ref="C76" r:id="rId75"/>
+    <hyperlink ref="C77" r:id="rId76"/>
+    <hyperlink ref="C78" r:id="rId77"/>
+    <hyperlink ref="C79" r:id="rId78"/>
+    <hyperlink ref="C80" r:id="rId79"/>
+    <hyperlink ref="C81" r:id="rId80"/>
+    <hyperlink ref="C82" r:id="rId81"/>
+    <hyperlink ref="C83" r:id="rId82"/>
+    <hyperlink ref="C84" r:id="rId83"/>
+    <hyperlink ref="C85" r:id="rId84"/>
+    <hyperlink ref="C86" r:id="rId85"/>
+    <hyperlink ref="C87" r:id="rId86"/>
+    <hyperlink ref="C88" r:id="rId87"/>
+    <hyperlink ref="C89" r:id="rId88"/>
+    <hyperlink ref="C90" r:id="rId89"/>
+    <hyperlink ref="C91" r:id="rId90"/>
+    <hyperlink ref="C92" r:id="rId91"/>
+    <hyperlink ref="C93" r:id="rId92"/>
+    <hyperlink ref="C94" r:id="rId93"/>
+    <hyperlink ref="C95" r:id="rId94"/>
+    <hyperlink ref="C96" r:id="rId95"/>
+    <hyperlink ref="C97" r:id="rId96"/>
+    <hyperlink ref="C98" r:id="rId97"/>
+    <hyperlink ref="C99" r:id="rId98"/>
+    <hyperlink ref="C100" r:id="rId99"/>
+    <hyperlink ref="C101" r:id="rId100"/>
+    <hyperlink ref="C102" r:id="rId101"/>
+    <hyperlink ref="C103" r:id="rId102"/>
+    <hyperlink ref="C104" r:id="rId103"/>
+    <hyperlink ref="C105" r:id="rId104"/>
+    <hyperlink ref="C106" r:id="rId105"/>
+    <hyperlink ref="C107" r:id="rId106"/>
+    <hyperlink ref="C108" r:id="rId107"/>
+    <hyperlink ref="C109" r:id="rId108"/>
+    <hyperlink ref="C110" r:id="rId109"/>
+    <hyperlink ref="C111" r:id="rId110"/>
+    <hyperlink ref="C112" r:id="rId111"/>
+    <hyperlink ref="C113" r:id="rId112"/>
+    <hyperlink ref="C114" r:id="rId113"/>
+    <hyperlink ref="C115" r:id="rId114"/>
+    <hyperlink ref="C116" r:id="rId115"/>
+    <hyperlink ref="C117" r:id="rId116"/>
+    <hyperlink ref="C118" r:id="rId117"/>
+    <hyperlink ref="C119" r:id="rId118"/>
+    <hyperlink ref="C120" r:id="rId119"/>
+    <hyperlink ref="C121" r:id="rId120"/>
+    <hyperlink ref="C122" r:id="rId121"/>
+    <hyperlink ref="C123" r:id="rId122"/>
+    <hyperlink ref="C124" r:id="rId123"/>
+    <hyperlink ref="C125" r:id="rId124"/>
+    <hyperlink ref="C126" r:id="rId125"/>
+    <hyperlink ref="C127" r:id="rId126"/>
+    <hyperlink ref="C128" r:id="rId127"/>
+    <hyperlink ref="C129" r:id="rId128"/>
+    <hyperlink ref="C130" r:id="rId129"/>
+    <hyperlink ref="C131" r:id="rId130"/>
+    <hyperlink ref="C132" r:id="rId131"/>
+    <hyperlink ref="C133" r:id="rId132"/>
+    <hyperlink ref="C134" r:id="rId133"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>